<commit_message>
Complete Guass Jordan Method
</commit_message>
<xml_diff>
--- a/Semaster 1/Introduction to Computer Science with Contemporary Language/Assignments/Guass Jordan Method/Gauss Jordan.xlsx
+++ b/Semaster 1/Introduction to Computer Science with Contemporary Language/Assignments/Guass Jordan Method/Gauss Jordan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1eb9d9405f58fdb/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UBIT\Semaster 1\Introduction to Computer Science with Contemporary Language\Assignments\Guass Jordan Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84FB7363-7A70-40AB-88CE-1944E42BDE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2235A239-9051-4235-B29A-8A7E59956E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7036F04B-9BC8-4D75-ABAB-D91D06395BE8}"/>
+    <workbookView xWindow="4575" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{7036F04B-9BC8-4D75-ABAB-D91D06395BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,20 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="23">
   <si>
     <t>solve system equation:</t>
   </si>
   <si>
-    <t xml:space="preserve">        eq1 --&gt; 2x-3y-5z = 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        eq2 --&gt; x-4y+z = -4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        eq3 --&gt; 6x+2y-3z = 5</t>
-  </si>
-  <si>
     <t>eq1</t>
   </si>
   <si>
@@ -98,17 +89,26 @@
     <t>Multiply R2 with inverse of (2,2)</t>
   </si>
   <si>
-    <t>Multiply additive inverse of (1, 2) with R2 and add it in R1</t>
-  </si>
-  <si>
-    <t>Multiply additive inverse of (0,2) with R2 and add it in R0</t>
+    <t xml:space="preserve">        eq1 --&gt; 4x -3y +z = -10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        eq2 --&gt; 2x+ y + 3z = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        eq3 --&gt; -x + 2y -5z =17</t>
+  </si>
+  <si>
+    <t>Multiply additive inverse of (0, 2) with R2 and add it in R0</t>
+  </si>
+  <si>
+    <t>Multiply additive inverse of (1,2) with R2 and add it in R1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +123,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF292C2E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -151,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -160,6 +167,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,428 +488,516 @@
   <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D4" si="0">AC30</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>4*D2-3*D3+D4</f>
+        <v>-10</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>2*D2+D3+3*D4</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E4">
+        <f>-D2+2*D3-5*D4</f>
+        <v>17</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Z8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>4</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
       </c>
       <c r="E9">
         <v>-3</v>
       </c>
       <c r="F9">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>-10</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O9">
+        <f t="shared" ref="O9:R11" si="1">D30</f>
         <v>1</v>
       </c>
       <c r="P9">
-        <v>-1.5</v>
+        <f t="shared" si="1"/>
+        <v>-0.75</v>
       </c>
       <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
         <v>-2.5</v>
       </c>
-      <c r="R9">
-        <v>3.5</v>
-      </c>
       <c r="Y9" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z9">
+        <f t="shared" ref="Z9:AC11" si="2">O30</f>
         <v>1</v>
       </c>
       <c r="AA9">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB9">
-        <v>-4.5999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P10">
-        <v>-2.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="Q10">
-        <v>3.5</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
       <c r="R10">
-        <v>-7.5</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Z10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA10">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB10">
-        <v>-1.4000000000000001</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O11">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P11">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>1.25</v>
       </c>
       <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>-4.75</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="2"/>
         <v>12</v>
-      </c>
-      <c r="R11">
-        <v>-16</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>27.400000000000002</v>
-      </c>
-      <c r="AC11">
-        <v>-49</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Z15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <f>2*(1/D9)</f>
+        <f>D9*(1/D9)</f>
         <v>1</v>
       </c>
       <c r="E16">
-        <f>-3*(1/D9)</f>
-        <v>-1.5</v>
+        <f>E9*(1/D9)</f>
+        <v>-0.75</v>
       </c>
       <c r="F16">
-        <f>-5*(1/D9)</f>
+        <f>F9*(1/D9)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G16">
+        <f>G9*(1/D9)</f>
         <v>-2.5</v>
       </c>
-      <c r="G16">
-        <f>7*(1/D9)</f>
-        <v>3.5</v>
-      </c>
       <c r="N16" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O16">
+        <f t="shared" ref="O16:R16" si="3">O9</f>
         <v>1</v>
       </c>
       <c r="P16">
-        <v>-1.5</v>
+        <f t="shared" si="3"/>
+        <v>-0.75</v>
       </c>
       <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
         <v>-2.5</v>
       </c>
-      <c r="R16">
-        <v>3.5</v>
-      </c>
       <c r="Y16" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z16">
+        <f t="shared" ref="Z16:AC17" si="4">Z9</f>
         <v>1</v>
       </c>
       <c r="AA16">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <v>-4.5999999999999996</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="AC16">
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <f t="shared" ref="D17:G18" si="5">D10</f>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>-4</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>-4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O17">
-        <f>0*(1/P10)</f>
+        <f>O10*(1/P10)</f>
         <v>0</v>
       </c>
       <c r="P17">
-        <f>-2.5*(1/P10)</f>
+        <f>P10*(1/P10)</f>
         <v>1</v>
       </c>
       <c r="Q17">
-        <f>3.5*(1/P10)</f>
-        <v>-1.4000000000000001</v>
+        <f>Q10*(1/P10)</f>
+        <v>1</v>
       </c>
       <c r="R17">
-        <f>-7.5*(1/P10)</f>
-        <v>3</v>
+        <f>R10*(1/P10)</f>
+        <v>2</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Z17">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA17">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AB17">
-        <v>-1.4000000000000001</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="AC17">
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>-1</v>
       </c>
       <c r="E18">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="F18">
-        <v>-3</v>
+        <f t="shared" si="5"/>
+        <v>-5</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O18">
+        <f t="shared" ref="O18:R18" si="6">O11</f>
         <v>0</v>
       </c>
       <c r="P18">
-        <v>11</v>
+        <f t="shared" si="6"/>
+        <v>1.25</v>
       </c>
       <c r="Q18">
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>-4.75</v>
       </c>
       <c r="R18">
-        <v>-16</v>
+        <f t="shared" si="6"/>
+        <v>14.5</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z18">
-        <f>0*(1/AB11)</f>
+        <f>Z11*(1/AB11)</f>
         <v>0</v>
       </c>
       <c r="AA18">
-        <f>0*(1/AB11)</f>
+        <f>AA11*(1/AB11)</f>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f>27.4*(1/AB11)</f>
-        <v>0.99999999999999989</v>
+        <f>AB11*(1/AB11)</f>
+        <v>1</v>
       </c>
       <c r="AC18">
-        <v>-49</v>
+        <f>AC11*(1/AB11)</f>
+        <v>-2</v>
       </c>
     </row>
     <row r="21" spans="3:34" x14ac:dyDescent="0.25">
       <c r="E21" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AA21" s="2" t="s">
         <v>21</v>
@@ -906,285 +1005,321 @@
     </row>
     <row r="22" spans="3:34" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Z22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="23" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23">
+        <f t="shared" ref="D23:G23" si="7">D16</f>
         <v>1</v>
       </c>
       <c r="E23">
-        <v>-1.5</v>
+        <f t="shared" si="7"/>
+        <v>-0.75</v>
       </c>
       <c r="F23">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
         <v>-2.5</v>
       </c>
-      <c r="G23">
-        <v>3.5</v>
-      </c>
       <c r="I23">
-        <f>-$D17*D23</f>
+        <f>-$D17*D16</f>
+        <v>-2</v>
+      </c>
+      <c r="J23">
+        <f>-$D17*E16</f>
+        <v>1.5</v>
+      </c>
+      <c r="K23">
+        <f>-$D17*F16</f>
+        <v>-0.5</v>
+      </c>
+      <c r="L23">
+        <f>-$D17*G16</f>
+        <v>5</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:R23" si="8">T24</f>
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
-      <c r="J23">
-        <f t="shared" ref="J23:L23" si="0">-$D17*E23</f>
+      <c r="T23">
+        <f>-$P16*O17</f>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f>-$P16*P17</f>
+        <v>0.75</v>
+      </c>
+      <c r="V23">
+        <f>-$P16*Q17</f>
+        <v>0.75</v>
+      </c>
+      <c r="W23">
+        <f>-$P16*R17</f>
         <v>1.5</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
-        <v>-3.5</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>-4.5999999999999996</v>
-      </c>
-      <c r="R23">
-        <v>8</v>
-      </c>
-      <c r="T23">
-        <f>-$P16*O24</f>
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <f t="shared" ref="U23:W23" si="1">-$P16*P24</f>
-        <v>1.5</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="1"/>
-        <v>-2.1</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
-      </c>
       <c r="Y23" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z23">
+        <f t="shared" ref="Z23:AC23" si="9">AE24</f>
         <v>1</v>
       </c>
       <c r="AA23">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB23">
-        <v>-4.5999999999999996</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AC23">
-        <v>8</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="AE23">
-        <f>-$AB17*Z25</f>
+        <f>-$AB16*Z18</f>
         <v>0</v>
       </c>
       <c r="AF23">
-        <f t="shared" ref="AF23:AH23" si="2">-$AB17*AA25</f>
+        <f>-$AB16*AA18</f>
         <v>0</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="2"/>
-        <v>1.4</v>
+        <f>-$AB16*AB18</f>
+        <v>-1</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="2"/>
-        <v>-68.600000000000009</v>
+        <f>-$AB16*AC18</f>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24">
+        <f t="shared" ref="D24:G24" si="10">I24</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <v>-2.5</v>
+        <f t="shared" si="10"/>
+        <v>2.5</v>
       </c>
       <c r="F24">
-        <v>3.5</v>
+        <f t="shared" si="10"/>
+        <v>2.5</v>
       </c>
       <c r="G24">
-        <v>-7.5</v>
+        <f t="shared" si="10"/>
+        <v>5</v>
       </c>
       <c r="I24">
         <f>D17+I23</f>
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:L24" si="3">E17+J23</f>
-        <v>-2.5</v>
+        <f>E17+J23</f>
+        <v>2.5</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
-        <v>3.5</v>
+        <f>F17+K23</f>
+        <v>2.5</v>
       </c>
       <c r="L24">
-        <f t="shared" si="3"/>
-        <v>-7.5</v>
+        <f>G17+L23</f>
+        <v>5</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O24">
+        <f t="shared" ref="O24:R25" si="11">O17</f>
         <v>0</v>
       </c>
       <c r="P24">
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q24">
-        <v>-1.4000000000000001</v>
+        <f t="shared" si="11"/>
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>3</v>
+        <f t="shared" si="11"/>
+        <v>2</v>
       </c>
       <c r="T24">
         <f>O16+T23</f>
         <v>1</v>
       </c>
       <c r="U24">
-        <f t="shared" ref="U24:W24" si="4">P16+U23</f>
+        <f t="shared" ref="U24:W24" si="12">P16+U23</f>
         <v>0</v>
       </c>
       <c r="V24">
-        <f t="shared" si="4"/>
-        <v>-4.5999999999999996</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="W24">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f t="shared" si="12"/>
+        <v>-1</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Z24">
+        <f t="shared" ref="Z24:AC24" si="13">Z17</f>
         <v>0</v>
       </c>
       <c r="AA24">
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AB24">
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="AC24">
-        <v>-65.600000000000009</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="AE24">
-        <f>Z17+AE23</f>
-        <v>0</v>
+        <f>Z16+AE23</f>
+        <v>1</v>
       </c>
       <c r="AF24">
-        <f t="shared" ref="AF24:AH24" si="5">AA17+AF23</f>
-        <v>1</v>
+        <f>AA16+AF23</f>
+        <v>0</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="5"/>
+        <f>AB16+AG23</f>
         <v>0</v>
       </c>
       <c r="AH24">
-        <f t="shared" si="5"/>
-        <v>-65.600000000000009</v>
+        <f>AC16+AH23</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <f t="shared" ref="D25:G25" si="14">D18</f>
+        <v>-1</v>
       </c>
       <c r="E25">
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="F25">
-        <v>-3</v>
+        <f t="shared" si="14"/>
+        <v>-5</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <f t="shared" si="14"/>
+        <v>17</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O25">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <v>11</v>
+        <f t="shared" si="11"/>
+        <v>1.25</v>
       </c>
       <c r="Q25">
-        <v>12</v>
+        <f t="shared" si="11"/>
+        <v>-4.75</v>
       </c>
       <c r="R25">
-        <v>-16</v>
+        <f t="shared" si="11"/>
+        <v>14.5</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z25">
+        <f t="shared" ref="Z25:AC25" si="15">Z18</f>
         <v>0</v>
       </c>
       <c r="AA25">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB25">
-        <v>0.99999999999999989</v>
+        <f t="shared" si="15"/>
+        <v>1</v>
       </c>
       <c r="AC25">
-        <v>-49</v>
+        <f t="shared" si="15"/>
+        <v>-2</v>
       </c>
     </row>
     <row r="28" spans="3:34" x14ac:dyDescent="0.25">
       <c r="E28" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AA28" s="2" t="s">
         <v>22</v>
@@ -1192,277 +1327,313 @@
     </row>
     <row r="29" spans="3:34" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="O29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="Z29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC29" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="AA29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC29" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30">
+        <f t="shared" ref="D30:G31" si="16">D23</f>
         <v>1</v>
       </c>
       <c r="E30">
-        <v>-1.5</v>
+        <f t="shared" si="16"/>
+        <v>-0.75</v>
       </c>
       <c r="F30">
+        <f t="shared" si="16"/>
+        <v>0.25</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="16"/>
         <v>-2.5</v>
       </c>
-      <c r="G30">
-        <v>3.5</v>
-      </c>
       <c r="I30">
-        <f>-$D25*D30</f>
-        <v>-6</v>
+        <f>-$D25*D23</f>
+        <v>1</v>
       </c>
       <c r="J30">
-        <f t="shared" ref="J30:L30" si="6">-$D25*E30</f>
-        <v>9</v>
+        <f>-$D25*E23</f>
+        <v>-0.75</v>
       </c>
       <c r="K30">
-        <f t="shared" si="6"/>
-        <v>15</v>
+        <f>-$D25*F23</f>
+        <v>0.25</v>
       </c>
       <c r="L30">
-        <f t="shared" si="6"/>
-        <v>-21</v>
+        <f>-$D25*G23</f>
+        <v>-2.5</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O30">
+        <f t="shared" ref="O30:R31" si="17">O23</f>
         <v>1</v>
       </c>
       <c r="P30">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <v>-4.5999999999999996</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="R30">
-        <v>8</v>
+        <f t="shared" si="17"/>
+        <v>-1</v>
       </c>
       <c r="T30">
-        <f>-$P25*O31</f>
+        <f>-$P25*O24</f>
         <v>0</v>
       </c>
       <c r="U30">
-        <f t="shared" ref="U30:W30" si="7">-$P25*P31</f>
-        <v>-11</v>
+        <f>-$P25*P24</f>
+        <v>-1.25</v>
       </c>
       <c r="V30">
-        <f t="shared" si="7"/>
-        <v>15.400000000000002</v>
+        <f>-$P25*Q24</f>
+        <v>-1.25</v>
       </c>
       <c r="W30">
-        <f t="shared" si="7"/>
-        <v>-33</v>
+        <f>-$P25*R24</f>
+        <v>-2.5</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z30">
+        <f t="shared" ref="Z30:AC30" si="18">Z23</f>
         <v>1</v>
       </c>
       <c r="AA30">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AB30">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="AC30">
-        <v>-217.39999999999998</v>
+        <f t="shared" si="18"/>
+        <v>1</v>
       </c>
       <c r="AE30">
-        <f>-$AB23*Z25</f>
+        <f>-$AB24*Z25</f>
         <v>0</v>
       </c>
       <c r="AF30">
-        <f t="shared" ref="AF30:AH30" si="8">-$AB23*AA25</f>
+        <f>-$AB24*AA25</f>
         <v>0</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="8"/>
-        <v>4.5999999999999988</v>
+        <f>-$AB24*AB25</f>
+        <v>-1</v>
       </c>
       <c r="AH30">
-        <f t="shared" si="8"/>
-        <v>-225.39999999999998</v>
+        <f>-$AB24*AC25</f>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D31">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="E31">
-        <v>-2.5</v>
+        <f t="shared" si="16"/>
+        <v>2.5</v>
       </c>
       <c r="F31">
-        <v>3.5</v>
+        <f t="shared" si="16"/>
+        <v>2.5</v>
       </c>
       <c r="G31">
-        <v>-7.5</v>
+        <f t="shared" si="16"/>
+        <v>5</v>
       </c>
       <c r="I31">
         <f>D25+I30</f>
         <v>0</v>
       </c>
       <c r="J31">
-        <f t="shared" ref="J31:L31" si="9">E25+J30</f>
-        <v>11</v>
+        <f t="shared" ref="J31:L31" si="19">E25+J30</f>
+        <v>1.25</v>
       </c>
       <c r="K31">
-        <f t="shared" si="9"/>
-        <v>12</v>
+        <f t="shared" si="19"/>
+        <v>-4.75</v>
       </c>
       <c r="L31">
-        <f t="shared" si="9"/>
-        <v>-16</v>
+        <f t="shared" si="19"/>
+        <v>14.5</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O31">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="P31">
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="Q31">
-        <v>-1.4000000000000001</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="R31">
-        <v>3</v>
+        <f t="shared" si="17"/>
+        <v>2</v>
       </c>
       <c r="T31">
         <f>O25+T30</f>
         <v>0</v>
       </c>
       <c r="U31">
-        <f t="shared" ref="U31:W31" si="10">P25+U30</f>
+        <f t="shared" ref="U31:W31" si="20">P25+U30</f>
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" si="10"/>
-        <v>27.400000000000002</v>
+        <f t="shared" si="20"/>
+        <v>-6</v>
       </c>
       <c r="W31">
-        <f t="shared" si="10"/>
-        <v>-49</v>
+        <f t="shared" si="20"/>
+        <v>12</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Z31">
+        <f t="shared" ref="Z31:AC31" si="21">AE31</f>
         <v>0</v>
       </c>
       <c r="AA31">
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="AB31">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <v>-65.600000000000009</v>
+        <f t="shared" si="21"/>
+        <v>4</v>
       </c>
       <c r="AE31">
-        <f>Z23+AE30</f>
-        <v>1</v>
+        <f>Z24+AE30</f>
+        <v>0</v>
       </c>
       <c r="AF31">
-        <f t="shared" ref="AF31:AH31" si="11">AA23+AF30</f>
-        <v>0</v>
+        <f>AA24+AF30</f>
+        <v>1</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="11"/>
+        <f>AB24+AG30</f>
         <v>0</v>
       </c>
       <c r="AH31">
-        <f t="shared" si="11"/>
-        <v>-217.39999999999998</v>
+        <f>AC24+AH30</f>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="3:34" x14ac:dyDescent="0.25">
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D32">
+        <f t="shared" ref="D32:G32" si="22">I31</f>
         <v>0</v>
       </c>
       <c r="E32">
-        <v>11</v>
+        <f t="shared" si="22"/>
+        <v>1.25</v>
       </c>
       <c r="F32">
+        <f t="shared" si="22"/>
+        <v>-4.75</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="22"/>
+        <v>14.5</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ref="O32:R32" si="23">T31</f>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="23"/>
+        <v>-6</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="23"/>
         <v>12</v>
       </c>
-      <c r="G32">
-        <v>-16</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>27.400000000000002</v>
-      </c>
-      <c r="R32">
-        <v>-49</v>
-      </c>
       <c r="Y32" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z32">
+        <f t="shared" ref="Z31:AC32" si="24">Z25</f>
         <v>0</v>
       </c>
       <c r="AA32">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AB32">
-        <v>0.99999999999999989</v>
+        <f t="shared" si="24"/>
+        <v>1</v>
       </c>
       <c r="AC32">
-        <v>-49</v>
+        <f t="shared" si="24"/>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>